<commit_message>
New version updated on 24/4/22
</commit_message>
<xml_diff>
--- a/Data/Input/TESCO Shipment Schedule- 1 TO 30 APRIL.xlsx
+++ b/Data/Input/TESCO Shipment Schedule- 1 TO 30 APRIL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UiPath Project for SQ\Tesco Demico portal\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A961673-D971-4B2A-B1F6-1F1B692F954C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3667C3A9-BD89-4F48-A903-7EC3792F6752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21300" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment Schedule Report" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="268">
   <si>
     <t/>
   </si>
@@ -886,6 +886,9 @@
   </si>
   <si>
     <t>DESTINATION</t>
+  </si>
+  <si>
+    <t>120-09045</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1048,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1459,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H31" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,13 +1621,13 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="6" t="s">
         <v>37</v>
       </c>
@@ -1669,8 +1672,8 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="10" t="s">
         <v>24</v>
       </c>
@@ -1730,13 +1733,13 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
       <c r="H5" s="6" t="s">
         <v>42</v>
       </c>
@@ -1781,8 +1784,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="10" t="s">
         <v>43</v>
       </c>
@@ -1842,14 +1845,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="11"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1891,13 +1894,13 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="10" t="s">
         <v>50</v>
       </c>
@@ -1942,14 +1945,14 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="6" t="s">
         <v>41</v>
       </c>
@@ -1991,8 +1994,8 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="10" t="s">
         <v>43</v>
       </c>
@@ -2052,14 +2055,14 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="6" t="s">
         <v>41</v>
       </c>
@@ -2101,13 +2104,13 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="10" t="s">
         <v>56</v>
       </c>
@@ -2152,14 +2155,14 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="6" t="s">
         <v>41</v>
       </c>
@@ -2201,8 +2204,8 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
@@ -2262,14 +2265,14 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="11"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="6" t="s">
         <v>41</v>
       </c>
@@ -2311,13 +2314,13 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="10" t="s">
         <v>61</v>
       </c>
@@ -2362,14 +2365,14 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="6" t="s">
         <v>41</v>
       </c>
@@ -2411,8 +2414,8 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="24" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="10" t="s">
         <v>24</v>
       </c>
@@ -2472,14 +2475,14 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="24" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="6" t="s">
         <v>68</v>
       </c>
@@ -2521,14 +2524,14 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="6" t="s">
         <v>69</v>
       </c>
@@ -2570,8 +2573,8 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="6" t="s">
         <v>24</v>
       </c>
@@ -2631,8 +2634,8 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="6" t="s">
         <v>24</v>
       </c>
@@ -2692,8 +2695,8 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="6" t="s">
         <v>24</v>
       </c>
@@ -2753,8 +2756,8 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="6" t="s">
         <v>24</v>
       </c>
@@ -2814,8 +2817,8 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="6" t="s">
         <v>24</v>
       </c>
@@ -2875,8 +2878,8 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="6" t="s">
         <v>24</v>
       </c>
@@ -2936,8 +2939,8 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="10" t="s">
         <v>43</v>
       </c>
@@ -2997,14 +3000,14 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="6" t="s">
         <v>68</v>
       </c>
@@ -3046,14 +3049,14 @@
       </c>
     </row>
     <row r="29" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="6" t="s">
         <v>69</v>
       </c>
@@ -3095,8 +3098,8 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="10" t="s">
         <v>43</v>
       </c>
@@ -3156,14 +3159,14 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="6" t="s">
         <v>102</v>
       </c>
@@ -3205,14 +3208,14 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="6" t="s">
         <v>103</v>
       </c>
@@ -3254,8 +3257,8 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="6" t="s">
         <v>104</v>
       </c>
@@ -3315,8 +3318,8 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="6" t="s">
         <v>24</v>
       </c>
@@ -3376,8 +3379,8 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="6" t="s">
         <v>24</v>
       </c>
@@ -3437,8 +3440,8 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="6" t="s">
         <v>24</v>
       </c>
@@ -3498,8 +3501,8 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="10" t="s">
         <v>24</v>
       </c>
@@ -3559,14 +3562,14 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
       <c r="I38" s="6" t="s">
         <v>68</v>
       </c>
@@ -3608,14 +3611,14 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
       <c r="I39" s="6" t="s">
         <v>69</v>
       </c>
@@ -3657,8 +3660,8 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="10" t="s">
         <v>24</v>
       </c>
@@ -3718,14 +3721,14 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
       <c r="I41" s="6" t="s">
         <v>68</v>
       </c>
@@ -3767,14 +3770,14 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
       <c r="I42" s="6" t="s">
         <v>69</v>
       </c>
@@ -3816,8 +3819,8 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="10" t="s">
         <v>24</v>
       </c>
@@ -3877,14 +3880,14 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
       <c r="I44" s="6" t="s">
         <v>68</v>
       </c>
@@ -3926,14 +3929,14 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
       <c r="I45" s="6" t="s">
         <v>69</v>
       </c>
@@ -3975,8 +3978,8 @@
       </c>
     </row>
     <row r="46" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="10" t="s">
         <v>24</v>
       </c>
@@ -4036,14 +4039,14 @@
       </c>
     </row>
     <row r="47" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
       <c r="I47" s="6" t="s">
         <v>68</v>
       </c>
@@ -4085,14 +4088,14 @@
       </c>
     </row>
     <row r="48" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
       <c r="I48" s="6" t="s">
         <v>69</v>
       </c>
@@ -4134,8 +4137,8 @@
       </c>
     </row>
     <row r="49" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="10" t="s">
         <v>24</v>
       </c>
@@ -4195,14 +4198,14 @@
       </c>
     </row>
     <row r="50" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
       <c r="I50" s="6" t="s">
         <v>68</v>
       </c>
@@ -4244,14 +4247,14 @@
       </c>
     </row>
     <row r="51" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
       <c r="I51" s="6" t="s">
         <v>69</v>
       </c>
@@ -4293,8 +4296,8 @@
       </c>
     </row>
     <row r="52" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
       <c r="C52" s="10" t="s">
         <v>24</v>
       </c>
@@ -4354,14 +4357,14 @@
       </c>
     </row>
     <row r="53" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
       <c r="I53" s="6" t="s">
         <v>68</v>
       </c>
@@ -4403,14 +4406,14 @@
       </c>
     </row>
     <row r="54" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
       <c r="I54" s="6" t="s">
         <v>69</v>
       </c>
@@ -4452,8 +4455,8 @@
       </c>
     </row>
     <row r="55" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
       <c r="C55" s="10" t="s">
         <v>24</v>
       </c>
@@ -4513,14 +4516,14 @@
       </c>
     </row>
     <row r="56" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
       <c r="I56" s="6" t="s">
         <v>68</v>
       </c>
@@ -4562,14 +4565,14 @@
       </c>
     </row>
     <row r="57" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
       <c r="I57" s="6" t="s">
         <v>69</v>
       </c>
@@ -4611,8 +4614,8 @@
       </c>
     </row>
     <row r="58" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
       <c r="C58" s="6" t="s">
         <v>24</v>
       </c>
@@ -4672,8 +4675,8 @@
       </c>
     </row>
     <row r="59" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
       <c r="C59" s="6" t="s">
         <v>24</v>
       </c>
@@ -4733,8 +4736,8 @@
       </c>
     </row>
     <row r="60" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
       <c r="C60" s="10" t="s">
         <v>24</v>
       </c>
@@ -4794,13 +4797,13 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
       <c r="H61" s="6" t="s">
         <v>153</v>
       </c>
@@ -4845,8 +4848,8 @@
       </c>
     </row>
     <row r="62" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
       <c r="C62" s="10" t="s">
         <v>24</v>
       </c>
@@ -4906,13 +4909,13 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
       <c r="H63" s="6" t="s">
         <v>153</v>
       </c>
@@ -4957,8 +4960,8 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
       <c r="C64" s="10" t="s">
         <v>24</v>
       </c>
@@ -5018,13 +5021,13 @@
       </c>
     </row>
     <row r="65" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
       <c r="H65" s="6" t="s">
         <v>153</v>
       </c>
@@ -5069,8 +5072,8 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
       <c r="C66" s="10" t="s">
         <v>24</v>
       </c>
@@ -5130,13 +5133,13 @@
       </c>
     </row>
     <row r="67" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
       <c r="H67" s="6" t="s">
         <v>153</v>
       </c>
@@ -5181,8 +5184,8 @@
       </c>
     </row>
     <row r="68" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
       <c r="C68" s="10" t="s">
         <v>24</v>
       </c>
@@ -5242,13 +5245,13 @@
       </c>
     </row>
     <row r="69" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
       <c r="H69" s="6" t="s">
         <v>153</v>
       </c>
@@ -5293,8 +5296,8 @@
       </c>
     </row>
     <row r="70" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="11"/>
       <c r="C70" s="10" t="s">
         <v>24</v>
       </c>
@@ -5354,13 +5357,13 @@
       </c>
     </row>
     <row r="71" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
       <c r="H71" s="6" t="s">
         <v>153</v>
       </c>
@@ -5405,8 +5408,8 @@
       </c>
     </row>
     <row r="72" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
       <c r="C72" s="6" t="s">
         <v>24</v>
       </c>
@@ -5466,8 +5469,8 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
       <c r="C73" s="6" t="s">
         <v>24</v>
       </c>
@@ -5527,8 +5530,8 @@
       </c>
     </row>
     <row r="74" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
       <c r="C74" s="6" t="s">
         <v>24</v>
       </c>
@@ -5588,8 +5591,8 @@
       </c>
     </row>
     <row r="75" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
       <c r="C75" s="6" t="s">
         <v>24</v>
       </c>
@@ -5649,8 +5652,8 @@
       </c>
     </row>
     <row r="76" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
       <c r="C76" s="10" t="s">
         <v>24</v>
       </c>
@@ -5710,13 +5713,13 @@
       </c>
     </row>
     <row r="77" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
       <c r="H77" s="6" t="s">
         <v>153</v>
       </c>
@@ -5761,8 +5764,8 @@
       </c>
     </row>
     <row r="78" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="11"/>
       <c r="C78" s="10" t="s">
         <v>24</v>
       </c>
@@ -5822,13 +5825,13 @@
       </c>
     </row>
     <row r="79" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
+      <c r="A79" s="11"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
       <c r="H79" s="6" t="s">
         <v>153</v>
       </c>
@@ -5873,8 +5876,8 @@
       </c>
     </row>
     <row r="80" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="11"/>
       <c r="C80" s="10" t="s">
         <v>24</v>
       </c>
@@ -5934,13 +5937,13 @@
       </c>
     </row>
     <row r="81" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
+      <c r="A81" s="11"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
       <c r="H81" s="6" t="s">
         <v>153</v>
       </c>
@@ -5985,8 +5988,8 @@
       </c>
     </row>
     <row r="82" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
       <c r="C82" s="10" t="s">
         <v>24</v>
       </c>
@@ -6046,13 +6049,13 @@
       </c>
     </row>
     <row r="83" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
       <c r="H83" s="6" t="s">
         <v>153</v>
       </c>
@@ -6097,8 +6100,8 @@
       </c>
     </row>
     <row r="84" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
       <c r="C84" s="10" t="s">
         <v>24</v>
       </c>
@@ -6158,13 +6161,13 @@
       </c>
     </row>
     <row r="85" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
       <c r="H85" s="6" t="s">
         <v>153</v>
       </c>
@@ -6209,8 +6212,8 @@
       </c>
     </row>
     <row r="86" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
       <c r="C86" s="10" t="s">
         <v>24</v>
       </c>
@@ -6270,13 +6273,13 @@
       </c>
     </row>
     <row r="87" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
       <c r="H87" s="6" t="s">
         <v>153</v>
       </c>
@@ -6321,8 +6324,8 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
       <c r="C88" s="10" t="s">
         <v>24</v>
       </c>
@@ -6382,13 +6385,13 @@
       </c>
     </row>
     <row r="89" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
+      <c r="A89" s="11"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
       <c r="H89" s="6" t="s">
         <v>56</v>
       </c>
@@ -6433,8 +6436,8 @@
       </c>
     </row>
     <row r="90" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
       <c r="C90" s="6" t="s">
         <v>24</v>
       </c>
@@ -6494,8 +6497,8 @@
       </c>
     </row>
     <row r="91" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
       <c r="C91" s="10" t="s">
         <v>24</v>
       </c>
@@ -6555,13 +6558,13 @@
       </c>
     </row>
     <row r="92" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11"/>
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
       <c r="H92" s="6" t="s">
         <v>56</v>
       </c>
@@ -6606,8 +6609,8 @@
       </c>
     </row>
     <row r="93" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
+      <c r="A93" s="11"/>
+      <c r="B93" s="11"/>
       <c r="C93" s="6" t="s">
         <v>24</v>
       </c>
@@ -6667,8 +6670,8 @@
       </c>
     </row>
     <row r="94" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
       <c r="C94" s="10" t="s">
         <v>24</v>
       </c>
@@ -6728,13 +6731,13 @@
       </c>
     </row>
     <row r="95" spans="1:21" ht="48" x14ac:dyDescent="0.25">
-      <c r="A95" s="12"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
+      <c r="A95" s="11"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
       <c r="H95" s="6" t="s">
         <v>153</v>
       </c>
@@ -6779,8 +6782,8 @@
       </c>
     </row>
     <row r="96" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
+      <c r="A96" s="11"/>
+      <c r="B96" s="11"/>
       <c r="C96" s="10" t="s">
         <v>104</v>
       </c>
@@ -6840,13 +6843,13 @@
       </c>
     </row>
     <row r="97" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12"/>
-      <c r="G97" s="12"/>
+      <c r="A97" s="11"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
       <c r="H97" s="6" t="s">
         <v>214</v>
       </c>
@@ -6891,13 +6894,13 @@
       </c>
     </row>
     <row r="98" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
+      <c r="A98" s="11"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
       <c r="H98" s="6" t="s">
         <v>215</v>
       </c>
@@ -6942,8 +6945,8 @@
       </c>
     </row>
     <row r="99" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
+      <c r="A99" s="11"/>
+      <c r="B99" s="11"/>
       <c r="C99" s="6" t="s">
         <v>24</v>
       </c>
@@ -7003,8 +7006,8 @@
       </c>
     </row>
     <row r="100" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
-      <c r="B100" s="12"/>
+      <c r="A100" s="11"/>
+      <c r="B100" s="11"/>
       <c r="C100" s="10" t="s">
         <v>104</v>
       </c>
@@ -7064,13 +7067,13 @@
       </c>
     </row>
     <row r="101" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
+      <c r="A101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+      <c r="G101" s="11"/>
       <c r="H101" s="6" t="s">
         <v>221</v>
       </c>
@@ -7115,13 +7118,13 @@
       </c>
     </row>
     <row r="102" spans="1:21" ht="36" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
       <c r="H102" s="6" t="s">
         <v>222</v>
       </c>
@@ -7166,8 +7169,8 @@
       </c>
     </row>
     <row r="103" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
+      <c r="A103" s="11"/>
+      <c r="B103" s="11"/>
       <c r="C103" s="10" t="s">
         <v>43</v>
       </c>
@@ -7227,14 +7230,14 @@
       </c>
     </row>
     <row r="104" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="12"/>
+      <c r="A104" s="11"/>
+      <c r="B104" s="11"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+      <c r="G104" s="11"/>
+      <c r="H104" s="11"/>
       <c r="I104" s="6" t="s">
         <v>68</v>
       </c>
@@ -7276,14 +7279,14 @@
       </c>
     </row>
     <row r="105" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="12"/>
+      <c r="H105" s="12"/>
       <c r="I105" s="6" t="s">
         <v>69</v>
       </c>
@@ -7325,8 +7328,8 @@
       </c>
     </row>
     <row r="106" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="12"/>
-      <c r="B106" s="12"/>
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
       <c r="C106" s="10" t="s">
         <v>43</v>
       </c>
@@ -7386,14 +7389,14 @@
       </c>
     </row>
     <row r="107" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="12"/>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
-      <c r="G107" s="12"/>
-      <c r="H107" s="12"/>
+      <c r="A107" s="11"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
       <c r="I107" s="6" t="s">
         <v>68</v>
       </c>
@@ -7435,14 +7438,14 @@
       </c>
     </row>
     <row r="108" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="12"/>
-      <c r="B108" s="12"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="12"/>
+      <c r="G108" s="12"/>
+      <c r="H108" s="12"/>
       <c r="I108" s="6" t="s">
         <v>69</v>
       </c>
@@ -7484,8 +7487,8 @@
       </c>
     </row>
     <row r="109" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="12"/>
-      <c r="B109" s="12"/>
+      <c r="A109" s="11"/>
+      <c r="B109" s="11"/>
       <c r="C109" s="6" t="s">
         <v>43</v>
       </c>
@@ -7545,8 +7548,8 @@
       </c>
     </row>
     <row r="110" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12"/>
-      <c r="B110" s="12"/>
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
       <c r="C110" s="6" t="s">
         <v>43</v>
       </c>
@@ -7606,8 +7609,8 @@
       </c>
     </row>
     <row r="111" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="12"/>
-      <c r="B111" s="12"/>
+      <c r="A111" s="11"/>
+      <c r="B111" s="11"/>
       <c r="C111" s="10" t="s">
         <v>43</v>
       </c>
@@ -7667,14 +7670,14 @@
       </c>
     </row>
     <row r="112" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="12"/>
-      <c r="B112" s="12"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
-      <c r="G112" s="12"/>
-      <c r="H112" s="12"/>
+      <c r="A112" s="11"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
       <c r="I112" s="6" t="s">
         <v>68</v>
       </c>
@@ -7716,14 +7719,14 @@
       </c>
     </row>
     <row r="113" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="12"/>
-      <c r="B113" s="12"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
-      <c r="G113" s="11"/>
-      <c r="H113" s="11"/>
+      <c r="A113" s="11"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12"/>
       <c r="I113" s="6" t="s">
         <v>69</v>
       </c>
@@ -7765,8 +7768,8 @@
       </c>
     </row>
     <row r="114" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
+      <c r="A114" s="11"/>
+      <c r="B114" s="11"/>
       <c r="C114" s="6" t="s">
         <v>43</v>
       </c>
@@ -7826,8 +7829,8 @@
       </c>
     </row>
     <row r="115" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="12"/>
-      <c r="B115" s="12"/>
+      <c r="A115" s="11"/>
+      <c r="B115" s="11"/>
       <c r="C115" s="6" t="s">
         <v>43</v>
       </c>
@@ -7887,8 +7890,8 @@
       </c>
     </row>
     <row r="116" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="12"/>
-      <c r="B116" s="12"/>
+      <c r="A116" s="11"/>
+      <c r="B116" s="11"/>
       <c r="C116" s="10" t="s">
         <v>24</v>
       </c>
@@ -7948,14 +7951,14 @@
       </c>
     </row>
     <row r="117" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="12"/>
-      <c r="B117" s="12"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="11"/>
+      <c r="A117" s="11"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+      <c r="G117" s="12"/>
+      <c r="H117" s="12"/>
       <c r="I117" s="6" t="s">
         <v>68</v>
       </c>
@@ -7997,8 +8000,8 @@
       </c>
     </row>
     <row r="118" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="12"/>
-      <c r="B118" s="12"/>
+      <c r="A118" s="11"/>
+      <c r="B118" s="11"/>
       <c r="C118" s="10" t="s">
         <v>24</v>
       </c>
@@ -8058,14 +8061,14 @@
       </c>
     </row>
     <row r="119" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
-      <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+      <c r="G119" s="12"/>
+      <c r="H119" s="12"/>
       <c r="I119" s="6" t="s">
         <v>68</v>
       </c>
@@ -8107,8 +8110,8 @@
       </c>
     </row>
     <row r="120" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
       <c r="C120" s="10" t="s">
         <v>24</v>
       </c>
@@ -8168,14 +8171,14 @@
       </c>
     </row>
     <row r="121" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="11"/>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
-      <c r="G121" s="11"/>
-      <c r="H121" s="11"/>
+      <c r="A121" s="12"/>
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+      <c r="G121" s="12"/>
+      <c r="H121" s="12"/>
       <c r="I121" s="6" t="s">
         <v>68</v>
       </c>
@@ -8221,6 +8224,196 @@
   </sheetData>
   <autoFilter ref="A1:U121" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="214">
+    <mergeCell ref="H118:H119"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="H120:H121"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="H111:H113"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="G116:G117"/>
+    <mergeCell ref="H116:H117"/>
+    <mergeCell ref="C111:C113"/>
+    <mergeCell ref="D111:D113"/>
+    <mergeCell ref="E111:E113"/>
+    <mergeCell ref="F111:F113"/>
+    <mergeCell ref="G111:G113"/>
+    <mergeCell ref="H103:H105"/>
+    <mergeCell ref="C106:C108"/>
+    <mergeCell ref="D106:D108"/>
+    <mergeCell ref="E106:E108"/>
+    <mergeCell ref="F106:F108"/>
+    <mergeCell ref="G106:G108"/>
+    <mergeCell ref="H106:H108"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="D103:D105"/>
+    <mergeCell ref="E103:E105"/>
+    <mergeCell ref="F103:F105"/>
+    <mergeCell ref="G103:G105"/>
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="E96:E98"/>
+    <mergeCell ref="F96:F98"/>
+    <mergeCell ref="G96:G98"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="F94:F95"/>
+    <mergeCell ref="G94:G95"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="G88:G89"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="G84:G85"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="F80:F81"/>
+    <mergeCell ref="G80:G81"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="H52:H54"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="G55:G57"/>
+    <mergeCell ref="H55:H57"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="H46:H48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="H49:H51"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="H43:H45"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="F6:F9"/>
@@ -8245,196 +8438,6 @@
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="H40:H42"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="H43:H45"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H46:H48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="H49:H51"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="H52:H54"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="D55:D57"/>
-    <mergeCell ref="E55:E57"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="G55:G57"/>
-    <mergeCell ref="H55:H57"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="G76:G77"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="F80:F81"/>
-    <mergeCell ref="G80:G81"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="G78:G79"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="G84:G85"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="G88:G89"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="F94:F95"/>
-    <mergeCell ref="G94:G95"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="C100:C102"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="G100:G102"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="D96:D98"/>
-    <mergeCell ref="E96:E98"/>
-    <mergeCell ref="F96:F98"/>
-    <mergeCell ref="G96:G98"/>
-    <mergeCell ref="H103:H105"/>
-    <mergeCell ref="C106:C108"/>
-    <mergeCell ref="D106:D108"/>
-    <mergeCell ref="E106:E108"/>
-    <mergeCell ref="F106:F108"/>
-    <mergeCell ref="G106:G108"/>
-    <mergeCell ref="H106:H108"/>
-    <mergeCell ref="C103:C105"/>
-    <mergeCell ref="D103:D105"/>
-    <mergeCell ref="E103:E105"/>
-    <mergeCell ref="F103:F105"/>
-    <mergeCell ref="G103:G105"/>
-    <mergeCell ref="H111:H113"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="G116:G117"/>
-    <mergeCell ref="H116:H117"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="D111:D113"/>
-    <mergeCell ref="E111:E113"/>
-    <mergeCell ref="F111:F113"/>
-    <mergeCell ref="G111:G113"/>
-    <mergeCell ref="H118:H119"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="G120:G121"/>
-    <mergeCell ref="H120:H121"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="G118:G119"/>
   </mergeCells>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.196850393700787" bottom="0.50240590551181097" header="0.196850393700787" footer="0.196850393700787"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -8579,12 +8582,12 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="6" t="s">
         <v>68</v>
       </c>
@@ -8687,12 +8690,12 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="6" t="s">
         <v>68</v>
       </c>
@@ -8793,12 +8796,12 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="6" t="s">
         <v>68</v>
       </c>
@@ -8841,6 +8844,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -8853,12 +8862,6 @@
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8867,10 +8870,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB0B283-3CDE-4015-88F8-C81FF6217817}">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8943,33 +8946,33 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="108" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>150</v>
+        <v>106</v>
+      </c>
+      <c r="H2" t="s">
+        <v>267</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2">
-        <v>44669</v>
+        <v>44676</v>
       </c>
       <c r="K2" s="2">
-        <v>44669</v>
+        <v>44676</v>
       </c>
       <c r="L2" s="3">
-        <v>1962</v>
+        <v>1500</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N2" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="O2" s="8">
-        <v>0</v>
+        <v>1.17</v>
+      </c>
+      <c r="O2" s="5">
+        <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>32</v>
@@ -8978,7 +8981,7 @@
         <v>33</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>160</v>
+        <v>226</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>0</v>
@@ -8991,32 +8994,34 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" t="s">
-        <v>106</v>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>254</v>
       </c>
       <c r="H3" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>30</v>
+        <v>256</v>
       </c>
       <c r="J3" s="2">
-        <v>44676</v>
+        <v>44669</v>
       </c>
       <c r="K3" s="2">
-        <v>44676</v>
+        <v>44669</v>
       </c>
       <c r="L3" s="3">
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N3" s="4">
-        <v>1.17</v>
+        <v>1.0667</v>
       </c>
       <c r="O3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>32</v>
@@ -9025,229 +9030,15 @@
         <v>33</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="72" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="2">
-        <v>44669</v>
-      </c>
-      <c r="K4" s="2">
-        <v>44669</v>
-      </c>
-      <c r="L4" s="3">
-        <v>17500</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="O4" s="8">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" s="2">
-        <v>44676</v>
-      </c>
-      <c r="K5" s="2">
-        <v>44676</v>
-      </c>
-      <c r="L5" s="3">
-        <v>10500</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.63329999999999997</v>
-      </c>
-      <c r="O5" s="5">
-        <v>3</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="G6" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="H6" t="s">
-        <v>260</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="J6" s="2">
-        <v>44669</v>
-      </c>
-      <c r="K6" s="2">
-        <v>44669</v>
-      </c>
-      <c r="L6" s="3">
-        <v>4000</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="4">
-        <v>1.0667</v>
-      </c>
-      <c r="O6" s="5">
-        <v>2</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>227</v>
-      </c>
-      <c r="H7" t="s">
-        <v>229</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="2">
-        <v>44669</v>
-      </c>
-      <c r="K7" s="2">
-        <v>44669</v>
-      </c>
-      <c r="L7" s="3">
-        <v>1500</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="4">
-        <v>1.2534000000000001</v>
-      </c>
-      <c r="O7" s="5">
-        <v>1</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="U7" s="6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -9259,14 +9050,227 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B78851-C328-40D7-970B-6424562F5EEC}">
-  <dimension ref="A1"/>
+  <dimension ref="C1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="3:21" ht="108" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="2">
+        <v>44669</v>
+      </c>
+      <c r="K1" s="2">
+        <v>44669</v>
+      </c>
+      <c r="L1" s="3">
+        <v>1962</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="O1" s="8">
+        <v>0</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="3:21" ht="72" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2">
+        <v>44669</v>
+      </c>
+      <c r="K2" s="2">
+        <v>44669</v>
+      </c>
+      <c r="L2" s="3">
+        <v>17500</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="3:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="2">
+        <v>44676</v>
+      </c>
+      <c r="K3" s="2">
+        <v>44676</v>
+      </c>
+      <c r="L3" s="3">
+        <v>10500</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.63329999999999997</v>
+      </c>
+      <c r="O3" s="5">
+        <v>3</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="3:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2">
+        <v>44669</v>
+      </c>
+      <c r="K4" s="2">
+        <v>44669</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1500</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="4">
+        <v>1.2534000000000001</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>